<commit_message>
local commit for kqi branch
</commit_message>
<xml_diff>
--- a/data/577 Projects/2017-2018/file list_2017-2018.xlsx
+++ b/data/577 Projects/2017-2018/file list_2017-2018.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C12A7EF5-9EA7-4AEF-80C1-233AF7C9FF67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="21930" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>PROJ</t>
   </si>
@@ -70,30 +80,54 @@
   <si>
     <t>Scriptonomics</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> URL</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>D:\ResearchSpace\Repositories\577 projects\fall2017\projects\f17team01\Valuation</t>
+  </si>
+  <si>
+    <t>D:\ResearchSpace\Repositories\577 projects\fall2017\projects\f17team02\Foundations\DCP</t>
+  </si>
+  <si>
+    <t>D:\ResearchSpace\Repositories\577 projects\fall2017\projects\f17team03\Foundations</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>D:\ResearchSpace\Repositories\577 projects\fall2017\projects\f17team06\Valuation\TA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -145,7 +179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -161,7 +195,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -236,6 +270,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -271,6 +322,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,22 +514,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="80.28515625" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="5" width="25.7265625" customWidth="1"/>
+    <col min="6" max="6" width="80.26953125" customWidth="1"/>
+    <col min="7" max="7" width="48.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -471,11 +539,17 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -485,14 +559,16 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -502,8 +578,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2</v>
       </c>
@@ -513,8 +595,14 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>3</v>
       </c>
@@ -524,8 +612,14 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>4</v>
       </c>
@@ -535,8 +629,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>5</v>
       </c>
@@ -546,8 +643,11 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>6</v>
       </c>
@@ -557,8 +657,14 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>7</v>
       </c>
@@ -568,10 +674,15 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25"/>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="D11">
+        <v>2018</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>